<commit_message>
Bulk search added.(Dep and Level wise)
</commit_message>
<xml_diff>
--- a/minimal/exlupload/bill.xlsx
+++ b/minimal/exlupload/bill.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saqlain\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F89102-3148-4D37-AE21-FD9364391948}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08BE24D-CB61-4D53-8A00-5607522BFAA0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24240" windowHeight="12528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,7 +527,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>87</v>
+        <v>201514087</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added more bulk search options.
</commit_message>
<xml_diff>
--- a/minimal/exlupload/bill.xlsx
+++ b/minimal/exlupload/bill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saqlain\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08BE24D-CB61-4D53-8A00-5607522BFAA0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10060EA9-40E7-42BA-B581-06767EB7E2AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24240" windowHeight="12528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="8">
   <si>
     <t>Hall Bill</t>
   </si>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,8 +62,23 @@
     <font>
       <sz val="8"/>
       <color rgb="FF444444"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,11 +101,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,117 +447,389 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>201514001</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="2">
         <v>43344</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>5000</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>201514002</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>43313</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>5000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>201514003</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>43344</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>1500</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>201514004</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>20000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>201514005</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>3000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>201514087</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>43361</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
         <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>201516033</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43313</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>201515011</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43344</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>201516033</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43313</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>201516033</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43344</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>201516033</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>201516039</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>201516039</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>43361</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>201516046</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>43344</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>201516046</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>43313</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>201517022</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43344</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>201517022</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>201517066</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>201517066</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>43361</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>201517012</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>43344</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>201517012</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>43313</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>201515011</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>43344</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>